<commit_message>
Updating scripts for Pagination
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/pagination/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/pagination/TestData.xlsx
@@ -12,12 +12,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+  <si>
+    <t>Variable</t>
+  </si>
   <si>
     <t>Supported Browser Types</t>
   </si>
   <si>
-    <t>Variable</t>
+    <t>Data1</t>
+  </si>
+  <si>
+    <t>Data2</t>
+  </si>
+  <si>
+    <t>Data3</t>
+  </si>
+  <si>
+    <t>Data4</t>
+  </si>
+  <si>
+    <t>URLs</t>
   </si>
   <si>
     <t>MozillaFirefox</t>
@@ -32,21 +47,6 @@
     <t>MicrosoftEdge</t>
   </si>
   <si>
-    <t>Data1</t>
-  </si>
-  <si>
-    <t>Data2</t>
-  </si>
-  <si>
-    <t>Data3</t>
-  </si>
-  <si>
-    <t>Data4</t>
-  </si>
-  <si>
-    <t>URLs</t>
-  </si>
-  <si>
     <t>URL_login_login</t>
   </si>
   <si>
@@ -83,7 +83,28 @@
     <t>Password</t>
   </si>
   <si>
-    <t>C77296 - Chrome: Table Insight: Verify that the pagination UI is displayed correctly.</t>
+    <t>paginationDashboardName</t>
+  </si>
+  <si>
+    <t>Automation_Pivot_Pagination_Dashboard</t>
+  </si>
+  <si>
+    <t>paginationInsightName</t>
+  </si>
+  <si>
+    <t>Automation_Insight</t>
+  </si>
+  <si>
+    <t>paginationDashboardNamePageSize</t>
+  </si>
+  <si>
+    <t>Automation_Pagination_Dashboard_PageSize</t>
+  </si>
+  <si>
+    <t>PageSize</t>
+  </si>
+  <si>
+    <t>DefaultPageSize</t>
   </si>
 </sst>
 </file>
@@ -156,15 +177,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="2" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -179,6 +200,12 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -206,7 +233,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="27.86"/>
+    <col customWidth="1" min="1" max="1" width="31.14"/>
     <col customWidth="1" min="2" max="2" width="64.29"/>
     <col customWidth="1" min="3" max="3" width="36.14"/>
     <col customWidth="1" min="4" max="15" width="8.57"/>
@@ -214,45 +241,45 @@
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
     </row>
     <row r="2" ht="13.5" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
@@ -495,9 +522,7 @@
       <c r="Y9" s="7"/>
     </row>
     <row r="10" ht="13.5" customHeight="1">
-      <c r="A10" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
@@ -523,11 +548,46 @@
       <c r="X10" s="6"/>
       <c r="Y10" s="6"/>
     </row>
-    <row r="11" ht="13.5" customHeight="1"/>
-    <row r="12" ht="13.5" customHeight="1"/>
-    <row r="13" ht="13.5" customHeight="1"/>
-    <row r="14" ht="13.5" customHeight="1"/>
-    <row r="15" ht="13.5" customHeight="1"/>
+    <row r="11" ht="13.5" customHeight="1">
+      <c r="A11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" ht="13.5" customHeight="1">
+      <c r="A12" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" ht="13.5" customHeight="1">
+      <c r="A13" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" ht="13.5" customHeight="1">
+      <c r="A14" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="9">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="15" ht="13.5" customHeight="1">
+      <c r="A15" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="10">
+        <v>10000.0</v>
+      </c>
+    </row>
     <row r="16" ht="13.5" customHeight="1"/>
     <row r="17" ht="13.5" customHeight="1"/>
     <row r="18" ht="13.5" customHeight="1"/>
@@ -1543,129 +1603,129 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
updated scripts and functions.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/pagination/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/pagination/TestData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>Variable</t>
   </si>
@@ -105,6 +105,12 @@
   </si>
   <si>
     <t>DefaultPageSize</t>
+  </si>
+  <si>
+    <t>NonPositiveIntegerPageSize</t>
+  </si>
+  <si>
+    <t>PageSize5</t>
   </si>
 </sst>
 </file>
@@ -177,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -202,6 +208,9 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -576,7 +585,7 @@
       <c r="A14" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="10">
         <v>10.0</v>
       </c>
     </row>
@@ -584,12 +593,26 @@
       <c r="A15" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="11">
         <v>10000.0</v>
       </c>
     </row>
-    <row r="16" ht="13.5" customHeight="1"/>
-    <row r="17" ht="13.5" customHeight="1"/>
+    <row r="16" ht="13.5" customHeight="1">
+      <c r="A16" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="9">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="17" ht="13.5" customHeight="1">
+      <c r="A17" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="9">
+        <v>5.0</v>
+      </c>
+    </row>
     <row r="18" ht="13.5" customHeight="1"/>
     <row r="19" ht="13.5" customHeight="1"/>
     <row r="20" ht="13.5" customHeight="1"/>

</xml_diff>

<commit_message>
Re-factoring test cases and functions and updating TestData file.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/pagination/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/pagination/TestData.xlsx
@@ -183,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -208,9 +208,6 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -585,7 +582,7 @@
       <c r="A14" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="9">
         <v>10.0</v>
       </c>
     </row>
@@ -593,8 +590,8 @@
       <c r="A15" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="11">
-        <v>10000.0</v>
+      <c r="B15" s="10">
+        <v>1000.0</v>
       </c>
     </row>
     <row r="16" ht="13.5" customHeight="1">

</xml_diff>

<commit_message>
Updating function and TCs. AllContent_Dashboard: Updated function locator. AllContent_DashboardPagination: Updated TCs. TestData: Updating test data.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/pagination/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/pagination/TestData.xlsx
@@ -12,29 +12,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>Variable</t>
   </si>
   <si>
+    <t>Data1</t>
+  </si>
+  <si>
+    <t>Data2</t>
+  </si>
+  <si>
+    <t>Data3</t>
+  </si>
+  <si>
+    <t>Data4</t>
+  </si>
+  <si>
+    <t>URLs</t>
+  </si>
+  <si>
     <t>Supported Browser Types</t>
   </si>
   <si>
-    <t>Data1</t>
-  </si>
-  <si>
-    <t>Data2</t>
-  </si>
-  <si>
-    <t>Data3</t>
-  </si>
-  <si>
-    <t>Data4</t>
-  </si>
-  <si>
-    <t>URLs</t>
-  </si>
-  <si>
     <t>MozillaFirefox</t>
   </si>
   <si>
@@ -83,22 +83,16 @@
     <t>Password</t>
   </si>
   <si>
-    <t>paginationDashboardName</t>
-  </si>
-  <si>
-    <t>Automation_Pivot_Pagination_Dashboard</t>
-  </si>
-  <si>
     <t>paginationInsightName</t>
   </si>
   <si>
     <t>Automation_Insight</t>
   </si>
   <si>
-    <t>paginationDashboardNamePageSize</t>
-  </si>
-  <si>
-    <t>Automation_Pagination_Dashboard_PageSize</t>
+    <t>Automation_Pivot_PaginationDashboard_DefaultPageSize</t>
+  </si>
+  <si>
+    <t>Automation_Pivot_PaginationDashboard_PageSize20</t>
   </si>
   <si>
     <t>PageSize</t>
@@ -190,13 +184,13 @@
     <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf borderId="2" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -239,7 +233,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="31.14"/>
+    <col customWidth="1" min="1" max="1" width="49.71"/>
     <col customWidth="1" min="2" max="2" width="64.29"/>
     <col customWidth="1" min="3" max="3" width="36.14"/>
     <col customWidth="1" min="4" max="15" width="8.57"/>
@@ -251,16 +245,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -284,10 +278,10 @@
       <c r="Y1" s="1"/>
     </row>
     <row r="2" ht="13.5" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="4"/>
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3"/>
       <c r="C2" s="5"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -375,10 +369,10 @@
       <c r="Y4" s="7"/>
     </row>
     <row r="5" ht="13.5" customHeight="1">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="3"/>
       <c r="C5" s="5"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -528,8 +522,8 @@
       <c r="Y9" s="7"/>
     </row>
     <row r="10" ht="13.5" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -562,25 +556,25 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" ht="13.5" customHeight="1">
+    <row r="12">
       <c r="A12" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="9" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" ht="13.5" customHeight="1">
-      <c r="A13" s="9" t="s">
-        <v>27</v>
-      </c>
       <c r="B13" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="A14" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B14" s="9">
         <v>10.0</v>
@@ -588,7 +582,7 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="A15" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B15" s="10">
         <v>1000.0</v>
@@ -596,7 +590,7 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="A16" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B16" s="9">
         <v>-1.0</v>
@@ -604,17 +598,12 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="A17" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B17" s="9">
         <v>5.0</v>
       </c>
     </row>
-    <row r="18" ht="13.5" customHeight="1"/>
-    <row r="19" ht="13.5" customHeight="1"/>
-    <row r="20" ht="13.5" customHeight="1"/>
-    <row r="21" ht="13.5" customHeight="1"/>
-    <row r="22" ht="13.5" customHeight="1"/>
     <row r="23" ht="13.5" customHeight="1"/>
     <row r="24" ht="13.5" customHeight="1"/>
     <row r="25" ht="13.5" customHeight="1"/>
@@ -1623,129 +1612,129 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
+      <c r="A1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>